<commit_message>
Updated readmes of approach comm and lobbying
</commit_message>
<xml_diff>
--- a/Approach/2 - Lobbying/lobbying_climate_keywords.xlsx
+++ b/Approach/2 - Lobbying/lobbying_climate_keywords.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludov\Desktop\Thesis\Research itself\Step 3 - Design Development\2. Lobbying\Validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludov\Desktop\Thesis\Chapters\GitHub repository\Approach\2 - Lobbying\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE308DC6-F53F-4602-B2B2-FA09C76290E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37EF8FD-5751-46AF-A074-2011C036CC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="original list" sheetId="1" r:id="rId1"/>
-    <sheet name="final list" sheetId="2" r:id="rId2"/>
-    <sheet name="for table report" sheetId="3" r:id="rId3"/>
+    <sheet name="final list" sheetId="2" r:id="rId1"/>
+    <sheet name="for table report" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,24 +26,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={B6CD8F4D-C43D-4B66-981A-BA5B51AD6F25}</author>
-  </authors>
-  <commentList>
-    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{B6CD8F4D-C43D-4B66-981A-BA5B51AD6F25}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    These are to find if the companies discuss the United Nations Climate Change Conference or Conference of the Parties of the UNFCCC (COP number). So with these entries I want to include all the COPs</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={465B91EE-D8B7-41E8-A5FD-B44B39C1B1A6}</author>
@@ -71,7 +52,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={E4ADB250-F97C-4EF4-9304-F4ECD415CD9A}</author>
@@ -99,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="70">
   <si>
     <t>renewable electricity</t>
   </si>
@@ -116,9 +97,6 @@
     <t>renewable energy</t>
   </si>
   <si>
-    <t>carbon</t>
-  </si>
-  <si>
     <t>clean energy</t>
   </si>
   <si>
@@ -137,9 +115,6 @@
     <t>Original keywords</t>
   </si>
   <si>
-    <t>climate</t>
-  </si>
-  <si>
     <t>European Climate Law</t>
   </si>
   <si>
@@ -284,9 +259,6 @@
     <t>climate goal</t>
   </si>
   <si>
-    <t>climate policy, climate action, climate target</t>
-  </si>
-  <si>
     <t>net-zero</t>
   </si>
   <si>
@@ -309,12 +281,6 @@
   </si>
   <si>
     <t>climate policy, climate action, climate target, cliamate goals, climate policies, climate actions, climate targets</t>
-  </si>
-  <si>
-    <t>keywords removed in the final list</t>
-  </si>
-  <si>
-    <t>Legend:</t>
   </si>
   <si>
     <t>GROUP</t>
@@ -330,7 +296,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,25 +312,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -379,13 +333,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
@@ -678,20 +631,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A35" dT="2023-11-11T15:22:38.69" personId="{41D78081-484D-49D5-A1D4-80981FA5286D}" id="{B6CD8F4D-C43D-4B66-981A-BA5B51AD6F25}">
-    <text>These are to find if the companies discuss the United Nations Climate Change Conference or Conference of the Parties of the UNFCCC (COP number). So with these entries I want to include all the COPs</text>
-    <extLst>
-      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
-        <xltc2:checksum>2088407868</xltc2:checksum>
-        <xltc2:hyperlink startIndex="124" length="6" url="https://en.wikipedia.org/wiki/United_Nations_Framework_Convention_on_Climate_Change"/>
-      </x:ext>
-    </extLst>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2023-11-11T15:34:04.61" personId="{41D78081-484D-49D5-A1D4-80981FA5286D}" id="{465B91EE-D8B7-41E8-A5FD-B44B39C1B1A6}">
     <text>I removed "climate" and "carbon" because these are too general of keywords that could easily mean something else (they could thus have false positives).</text>
   </threadedComment>
@@ -707,7 +646,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2023-11-11T15:34:04.61" personId="{41D78081-484D-49D5-A1D4-80981FA5286D}" id="{E4ADB250-F97C-4EF4-9304-F4ECD415CD9A}">
     <text>I removed "climate" and "carbon" because these are too general of keywords that could easily mean something else (they could thus have false positives).</text>
@@ -725,11 +664,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5922127-A65B-41BE-96AE-FE9CEEC0232A}">
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,10 +678,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -752,7 +691,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -760,7 +699,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -773,10 +712,16 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -786,12 +731,15 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -801,51 +749,57 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -853,7 +807,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -861,7 +815,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -874,7 +828,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -884,15 +838,18 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -914,10 +871,16 @@
       <c r="A30" t="s">
         <v>33</v>
       </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -925,99 +888,76 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1027,331 +967,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5922127-A65B-41BE-96AE-FE9CEEC0232A}">
-  <dimension ref="A1:G41"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86C666D9-33CA-4746-8056-5BA737672530}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>29</v>
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1359,26 +996,26 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>41</v>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G4" s="2"/>
     </row>
@@ -1387,64 +1024,64 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>63</v>
+      <c r="B6" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>64</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>65</v>
+        <v>38</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1452,302 +1089,302 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>42</v>
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>43</v>
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>66</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>44</v>
+        <v>21</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>62</v>
+        <v>28</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>67</v>
+        <v>29</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>68</v>
+        <v>36</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>